<commit_message>
Fixed methods in anasyn.py
</commit_message>
<xml_diff>
--- a/docs/TablaAnalisis.xlsx
+++ b/docs/TablaAnalisis.xlsx
@@ -1535,8 +1535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AO127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A127" sqref="A127"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>

</xml_diff>

<commit_message>
corregido ; en tabla analasis y memoria
</commit_message>
<xml_diff>
--- a/docs/TablaAnalisis.xlsx
+++ b/docs/TablaAnalisis.xlsx
@@ -1,17 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elssbbboy/proclen/compilerProcesadoresLenguajesPractice4/docs/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="990"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="150001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
@@ -20,137 +30,137 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="96">
-  <si>
-    <t xml:space="preserve">PROGRAMA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VAR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VECTOR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[</t>
-  </si>
-  <si>
-    <t xml:space="preserve">]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">num</t>
-  </si>
-  <si>
-    <t xml:space="preserve">de</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ENTERO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BOOLEANO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PROC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FUNCION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INICIO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FIN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ENTONCES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SINO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MIENTRAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HACER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">opasigna</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LEE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ESCRIBE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(</t>
-  </si>
-  <si>
-    <t xml:space="preserve">)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">oprel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">opsuma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O</t>
-  </si>
-  <si>
-    <t xml:space="preserve">opmult</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CIERTO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;Programa&gt;</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">PROGRAMA id</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="96">
+  <si>
+    <t>PROGRAMA</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>;</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>VAR</t>
+  </si>
+  <si>
+    <t>:</t>
+  </si>
+  <si>
+    <t>,</t>
+  </si>
+  <si>
+    <t>VECTOR</t>
+  </si>
+  <si>
+    <t>[</t>
+  </si>
+  <si>
+    <t>]</t>
+  </si>
+  <si>
+    <t>num</t>
+  </si>
+  <si>
+    <t>de</t>
+  </si>
+  <si>
+    <t>ENTERO</t>
+  </si>
+  <si>
+    <t>REAL</t>
+  </si>
+  <si>
+    <t>BOOLEANO</t>
+  </si>
+  <si>
+    <t>PROC</t>
+  </si>
+  <si>
+    <t>FUNCION</t>
+  </si>
+  <si>
+    <t>INICIO</t>
+  </si>
+  <si>
+    <t>FIN</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>ENTONCES</t>
+  </si>
+  <si>
+    <t>SINO</t>
+  </si>
+  <si>
+    <t>MIENTRAS</t>
+  </si>
+  <si>
+    <t>HACER</t>
+  </si>
+  <si>
+    <t>opasigna</t>
+  </si>
+  <si>
+    <t>LEE</t>
+  </si>
+  <si>
+    <t>ESCRIBE</t>
+  </si>
+  <si>
+    <t>(</t>
+  </si>
+  <si>
+    <t>)</t>
+  </si>
+  <si>
+    <t>oprel</t>
+  </si>
+  <si>
+    <t>opsuma</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>opmult</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>CIERTO</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>$</t>
+  </si>
+  <si>
+    <t>&lt;Programa&gt;</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>PROGRAMA id</t>
     </r>
     <r>
       <rPr>
@@ -163,13 +173,13 @@
     </r>
     <r>
       <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">;</t>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>;</t>
     </r>
     <r>
       <rPr>
@@ -182,28 +192,28 @@
     </r>
     <r>
       <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;decl_var&gt;</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">VAR</t>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>&lt;decl_var&gt;</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>VAR</t>
     </r>
     <r>
       <rPr>
@@ -216,13 +226,13 @@
     </r>
     <r>
       <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">:</t>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>:</t>
     </r>
     <r>
       <rPr>
@@ -235,13 +245,13 @@
     </r>
     <r>
       <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">;</t>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>;</t>
     </r>
     <r>
       <rPr>
@@ -254,10 +264,10 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">λ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;decl_v&gt;</t>
+    <t>λ</t>
+  </si>
+  <si>
+    <t>&lt;decl_v&gt;</t>
   </si>
   <si>
     <r>
@@ -271,13 +281,13 @@
     </r>
     <r>
       <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">:</t>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>:</t>
     </r>
     <r>
       <rPr>
@@ -290,13 +300,13 @@
     </r>
     <r>
       <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">;</t>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>;</t>
     </r>
     <r>
       <rPr>
@@ -309,18 +319,18 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">&lt;lista_id&gt;</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">id</t>
+    <t>&lt;lista_id&gt;</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>id</t>
     </r>
     <r>
       <rPr>
@@ -333,18 +343,18 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">&lt;resto_listaid&gt;</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">,</t>
+    <t>&lt;resto_listaid&gt;</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>,</t>
     </r>
     <r>
       <rPr>
@@ -357,18 +367,18 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">&lt;tipo&gt;</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">VECTOR</t>
+    <t>&lt;tipo&gt;</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>VECTOR</t>
     </r>
     <r>
       <rPr>
@@ -381,13 +391,13 @@
     </r>
     <r>
       <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">[</t>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>[</t>
     </r>
     <r>
       <rPr>
@@ -400,13 +410,13 @@
     </r>
     <r>
       <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">num</t>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>num</t>
     </r>
     <r>
       <rPr>
@@ -419,13 +429,13 @@
     </r>
     <r>
       <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">]</t>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>]</t>
     </r>
     <r>
       <rPr>
@@ -438,13 +448,13 @@
     </r>
     <r>
       <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">de</t>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>de</t>
     </r>
     <r>
       <rPr>
@@ -457,10 +467,10 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">&lt;tipo_std&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;decl_subprg&gt;</t>
+    <t>&lt;tipo_std&gt;</t>
+  </si>
+  <si>
+    <t>&lt;decl_subprg&gt;</t>
   </si>
   <si>
     <r>
@@ -474,13 +484,13 @@
     </r>
     <r>
       <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">;</t>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>;</t>
     </r>
     <r>
       <rPr>
@@ -493,18 +503,18 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">&lt;decl_sub&gt;</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">PROC</t>
+    <t>&lt;decl_sub&gt;</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>PROC</t>
     </r>
     <r>
       <rPr>
@@ -517,13 +527,13 @@
     </r>
     <r>
       <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">id</t>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>id</t>
     </r>
     <r>
       <rPr>
@@ -536,13 +546,13 @@
     </r>
     <r>
       <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">;</t>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>;</t>
     </r>
     <r>
       <rPr>
@@ -557,13 +567,13 @@
   <si>
     <r>
       <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">FUNCION</t>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>FUNCION</t>
     </r>
     <r>
       <rPr>
@@ -576,13 +586,13 @@
     </r>
     <r>
       <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">id</t>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>id</t>
     </r>
     <r>
       <rPr>
@@ -595,13 +605,13 @@
     </r>
     <r>
       <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">:</t>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>:</t>
     </r>
     <r>
       <rPr>
@@ -614,13 +624,13 @@
     </r>
     <r>
       <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">;</t>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>;</t>
     </r>
     <r>
       <rPr>
@@ -633,18 +643,18 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">&lt;instrucciones&gt;</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">INICIO</t>
+    <t>&lt;instrucciones&gt;</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>INICIO</t>
     </r>
     <r>
       <rPr>
@@ -657,17 +667,17 @@
     </r>
     <r>
       <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">FIN</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;lista_inst&gt;</t>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>FIN</t>
+    </r>
+  </si>
+  <si>
+    <t>&lt;lista_inst&gt;</t>
   </si>
   <si>
     <r>
@@ -681,13 +691,13 @@
     </r>
     <r>
       <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">;</t>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>;</t>
     </r>
     <r>
       <rPr>
@@ -700,21 +710,21 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">&lt;instruccion&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;inst_simple&gt;</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">SI</t>
+    <t>&lt;instruccion&gt;</t>
+  </si>
+  <si>
+    <t>&lt;inst_simple&gt;</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>MIENTRAS</t>
     </r>
     <r>
       <rPr>
@@ -727,32 +737,13 @@
     </r>
     <r>
       <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">ENTONCES</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> &lt;instruccion&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">SINO</t>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>HACER</t>
     </r>
     <r>
       <rPr>
@@ -765,15 +756,437 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">MIENTRAS</t>
+    <t>&lt;inst_e/s&gt;</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;resto_instsimple&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>&lt;resto_instsimple&gt;</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;expr_simple&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>opasigna</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;expresion&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>opasigna</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;expresion&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>&lt;variable&gt;</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;resto_var&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>&lt;resto_var&gt;</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;expr_simple&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>LEE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>ESCRIBE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;expr_simple&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>&lt;expresion&gt;</t>
+  </si>
+  <si>
+    <t>&lt;expr_simple&gt; &lt;expr_aux&gt;</t>
+  </si>
+  <si>
+    <t>&lt;expr_aux&gt;</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>oprel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;expr_simple&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>&lt;expr_simple&gt;</t>
+  </si>
+  <si>
+    <t>&lt;termino&gt; &lt;resto_exsimple&gt;</t>
+  </si>
+  <si>
+    <t>&lt;signo&gt; &lt;termino&gt; &lt;resto_exsimple&gt;</t>
+  </si>
+  <si>
+    <t>&lt;resto_exsimple&gt;</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>opsuma</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;termino&gt; &lt;resto_exsimple&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>O</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;termino&gt; &lt;resto_exsimple&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>&lt;termino&gt;</t>
+  </si>
+  <si>
+    <t>&lt;factor&gt; &lt;resto_term&gt;</t>
+  </si>
+  <si>
+    <t>&lt;resto_term&gt;</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>opmult</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;factor&gt; &lt;resto_term&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Y</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;factor&gt; &lt;resto_term&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>&lt;factor&gt;</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>(</t>
     </r>
     <r>
       <rPr>
@@ -786,13 +1199,80 @@
     </r>
     <r>
       <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">HACER</t>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>NO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;factor&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>&lt;signo&gt;</t>
+  </si>
+  <si>
+    <r>
+      <t>SI</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;expresion&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>ENTONCES</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;instruccion&gt; ; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>SINO</t>
     </r>
     <r>
       <rPr>
@@ -803,495 +1283,16 @@
       </rPr>
       <t xml:space="preserve"> &lt;instruccion&gt;</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;inst_e/s&gt;</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">id</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> &lt;resto_instsimple&gt;</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;resto_instsimple&gt;</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> &lt;expr_simple&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">opasigna</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> &lt;expresion&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">opasigna</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> &lt;expresion&gt;</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;variable&gt;</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">id</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> &lt;resto_var&gt;</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;resto_var&gt;</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> &lt;expr_simple&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">LEE</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">id</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">ESCRIBE</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> &lt;expr_simple&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">)</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;expresion&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;expr_simple&gt; &lt;expr_aux&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;expr_aux&gt;</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">oprel</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> &lt;expr_simple&gt;</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;expr_simple&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;termino&gt; &lt;resto_exsimple&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;signo&gt; &lt;termino&gt; &lt;resto_exsimple&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;resto_exsimple&gt;</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">opsuma</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> &lt;termino&gt; &lt;resto_exsimple&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">O</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> &lt;termino&gt; &lt;resto_exsimple&gt;</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;termino&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;factor&gt; &lt;resto_term&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;resto_term&gt;</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">opmult</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> &lt;factor&gt; &lt;resto_term&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Y</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> &lt;factor&gt; &lt;resto_term&gt;</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;factor&gt;</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> &lt;expresion&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">NO</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> &lt;factor&gt;</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;signo&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="&quot;VERDADERO&quot;;&quot;VERDADERO&quot;;&quot;FALSO&quot;"/>
-    <numFmt numFmtId="166" formatCode="&quot;VERDADERO&quot;;&quot;VERDADERO&quot;;&quot;FALSO&quot;"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;VERDADERO&quot;;&quot;VERDADERO&quot;;&quot;FALSO&quot;"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1299,22 +1300,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -1330,148 +1316,351 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="DengXian"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO127"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E101" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G123" activeCellId="0" sqref="G123"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="W1" sqref="W1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.7040816326531"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.1479591836735"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="53.0510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="40.765306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.2908163265306"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="34.6938775510204"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="32.8010204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="35.3673469387755"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="28.3469387755102"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="24.1632653061224"/>
-    <col collapsed="false" hidden="false" max="16" min="13" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="36.8520408163265"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="53.1887755102041"/>
-    <col collapsed="false" hidden="false" max="23" min="22" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="40.3622448979592"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="24.3010204081633"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="24.3010204081633"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="32.8010204081633"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="28.0765306122449"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="27.2704081632653"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="24.7040816326531"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="26.0510204081633"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="31.7244897959184"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="32.9387755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="41" style="0" width="11.3418367346939"/>
+    <col min="4" max="4" width="32.83203125" customWidth="1"/>
+    <col min="5" max="5" width="43.83203125" customWidth="1"/>
+    <col min="21" max="21" width="55.33203125" customWidth="1"/>
+    <col min="22" max="22" width="13" customWidth="1"/>
+    <col min="23" max="23" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1581,8 +1770,8 @@
       <c r="AK1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AL1" s="3" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="AL1" s="3" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="AM1" s="2" t="s">
@@ -1595,7 +1784,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>39</v>
       </c>
@@ -1642,7 +1831,7 @@
       <c r="AN2" s="1"/>
       <c r="AO2" s="1"/>
     </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>41</v>
       </c>
@@ -1695,7 +1884,7 @@
       <c r="AN3" s="1"/>
       <c r="AO3" s="1"/>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>44</v>
       </c>
@@ -1748,7 +1937,7 @@
       <c r="AN4" s="1"/>
       <c r="AO4" s="1"/>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>46</v>
       </c>
@@ -1795,7 +1984,7 @@
       <c r="AN5" s="1"/>
       <c r="AO5" s="1"/>
     </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>48</v>
       </c>
@@ -1844,7 +2033,7 @@
       <c r="AN6" s="1"/>
       <c r="AO6" s="1"/>
     </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>50</v>
       </c>
@@ -1897,7 +2086,7 @@
       <c r="AN7" s="1"/>
       <c r="AO7" s="1"/>
     </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>52</v>
       </c>
@@ -1948,7 +2137,7 @@
       <c r="AN8" s="1"/>
       <c r="AO8" s="1"/>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>53</v>
       </c>
@@ -1999,7 +2188,7 @@
       <c r="AN9" s="1"/>
       <c r="AO9" s="1"/>
     </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>55</v>
       </c>
@@ -2048,7 +2237,7 @@
       <c r="AN10" s="1"/>
       <c r="AO10" s="1"/>
     </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>58</v>
       </c>
@@ -2095,7 +2284,7 @@
       <c r="AN11" s="1"/>
       <c r="AO11" s="1"/>
     </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>60</v>
       </c>
@@ -2154,7 +2343,7 @@
       <c r="AN12" s="1"/>
       <c r="AO12" s="1"/>
     </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>62</v>
       </c>
@@ -2182,20 +2371,20 @@
       </c>
       <c r="T13" s="1"/>
       <c r="U13" s="2" t="s">
-        <v>64</v>
+        <v>95</v>
       </c>
       <c r="V13" s="1"/>
       <c r="W13" s="1"/>
       <c r="X13" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
       <c r="AA13" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AB13" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AC13" s="1"/>
       <c r="AD13" s="1"/>
@@ -2211,13 +2400,13 @@
       <c r="AN13" s="1"/>
       <c r="AO13" s="1"/>
     </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -2258,9 +2447,9 @@
       <c r="AN14" s="1"/>
       <c r="AO14" s="1"/>
     </row>
-    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -2273,7 +2462,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
@@ -2287,13 +2476,11 @@
       <c r="T15" s="1"/>
       <c r="U15" s="1"/>
       <c r="V15" s="1"/>
-      <c r="W15" s="1" t="s">
-        <v>43</v>
-      </c>
+      <c r="W15" s="1"/>
       <c r="X15" s="1"/>
       <c r="Y15" s="1"/>
       <c r="Z15" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AA15" s="1"/>
       <c r="AB15" s="1"/>
@@ -2311,13 +2498,13 @@
       <c r="AN15" s="1"/>
       <c r="AO15" s="1"/>
     </row>
-    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -2358,9 +2545,9 @@
       <c r="AN16" s="1"/>
       <c r="AO16" s="1"/>
     </row>
-    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -2373,7 +2560,7 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>43</v>
@@ -2391,9 +2578,7 @@
       <c r="V17" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="W17" s="1" t="s">
-        <v>43</v>
-      </c>
+      <c r="W17" s="1"/>
       <c r="X17" s="1"/>
       <c r="Y17" s="1" t="s">
         <v>43</v>
@@ -2427,9 +2612,9 @@
       <c r="AN17" s="1"/>
       <c r="AO17" s="1"/>
     </row>
-    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -2457,10 +2642,10 @@
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
       <c r="AA18" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB18" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="AB18" s="2" t="s">
-        <v>76</v>
       </c>
       <c r="AC18" s="1"/>
       <c r="AD18" s="1"/>
@@ -2476,13 +2661,13 @@
       <c r="AN18" s="1"/>
       <c r="AO18" s="1"/>
     </row>
-    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -2493,7 +2678,7 @@
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
@@ -2512,7 +2697,7 @@
       <c r="AA19" s="1"/>
       <c r="AB19" s="1"/>
       <c r="AC19" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AD19" s="1"/>
       <c r="AE19" s="1"/>
@@ -2521,25 +2706,25 @@
       <c r="AH19" s="1"/>
       <c r="AI19" s="1"/>
       <c r="AJ19" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AK19" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AL19" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AM19" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AN19" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AO19" s="1"/>
+    </row>
+    <row r="20" spans="1:41" x14ac:dyDescent="0.15">
+      <c r="A20" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="AK19" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AL19" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AM19" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AN19" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AO19" s="1"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -2566,9 +2751,7 @@
       <c r="V20" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="W20" s="1" t="s">
-        <v>43</v>
-      </c>
+      <c r="W20" s="1"/>
       <c r="X20" s="1"/>
       <c r="Y20" s="1" t="s">
         <v>43</v>
@@ -2581,7 +2764,7 @@
         <v>43</v>
       </c>
       <c r="AE20" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AF20" s="1"/>
       <c r="AG20" s="1"/>
@@ -2594,13 +2777,13 @@
       <c r="AN20" s="1"/>
       <c r="AO20" s="1"/>
     </row>
-    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -2611,7 +2794,7 @@
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
@@ -2630,7 +2813,7 @@
       <c r="AA21" s="1"/>
       <c r="AB21" s="1"/>
       <c r="AC21" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AD21" s="1"/>
       <c r="AE21" s="1"/>
@@ -2639,25 +2822,25 @@
       <c r="AH21" s="1"/>
       <c r="AI21" s="1"/>
       <c r="AJ21" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AK21" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AL21" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AM21" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="AK21" s="1" t="s">
+      <c r="AN21" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="AL21" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AM21" s="1" t="s">
+      <c r="AO21" s="1"/>
+    </row>
+    <row r="22" spans="1:41" x14ac:dyDescent="0.15">
+      <c r="A22" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="AN21" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AO21" s="1"/>
-    </row>
-    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -2686,9 +2869,7 @@
       <c r="V22" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="W22" s="1" t="s">
-        <v>43</v>
-      </c>
+      <c r="W22" s="1"/>
       <c r="X22" s="1"/>
       <c r="Y22" s="1" t="s">
         <v>43</v>
@@ -2704,10 +2885,10 @@
         <v>43</v>
       </c>
       <c r="AF22" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="AG22" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="AG22" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="AH22" s="1"/>
       <c r="AI22" s="1"/>
@@ -2718,13 +2899,13 @@
       <c r="AN22" s="1"/>
       <c r="AO22" s="1"/>
     </row>
-    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -2735,7 +2916,7 @@
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
@@ -2754,7 +2935,7 @@
       <c r="AA23" s="1"/>
       <c r="AB23" s="1"/>
       <c r="AC23" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AD23" s="1"/>
       <c r="AE23" s="1"/>
@@ -2763,21 +2944,21 @@
       <c r="AH23" s="1"/>
       <c r="AI23" s="1"/>
       <c r="AJ23" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AK23" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AL23" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AM23" s="1"/>
       <c r="AN23" s="1"/>
       <c r="AO23" s="1"/>
     </row>
-    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -2806,9 +2987,7 @@
       <c r="V24" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="W24" s="1" t="s">
-        <v>43</v>
-      </c>
+      <c r="W24" s="1"/>
       <c r="X24" s="1"/>
       <c r="Y24" s="1" t="s">
         <v>43</v>
@@ -2830,10 +3009,10 @@
         <v>43</v>
       </c>
       <c r="AH24" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="AI24" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="AI24" s="2" t="s">
-        <v>91</v>
       </c>
       <c r="AJ24" s="1"/>
       <c r="AK24" s="1"/>
@@ -2842,13 +3021,13 @@
       <c r="AN24" s="1"/>
       <c r="AO24" s="1"/>
     </row>
-    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -2878,7 +3057,7 @@
       <c r="AA25" s="1"/>
       <c r="AB25" s="1"/>
       <c r="AC25" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AD25" s="1"/>
       <c r="AE25" s="1"/>
@@ -2887,22 +3066,22 @@
       <c r="AH25" s="1"/>
       <c r="AI25" s="1"/>
       <c r="AJ25" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AK25" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AL25" s="2" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="AL25" s="2" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="AM25" s="1"/>
       <c r="AN25" s="1"/>
       <c r="AO25" s="1"/>
     </row>
-    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -2949,7 +3128,7 @@
       </c>
       <c r="AO26" s="1"/>
     </row>
-    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A30" s="1"/>
       <c r="B30" s="2" t="s">
         <v>0</v>
@@ -2994,7 +3173,7 @@
       <c r="AN30" s="5"/>
       <c r="AO30" s="5"/>
     </row>
-    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:41" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
         <v>39</v>
       </c>
@@ -3041,7 +3220,7 @@
       <c r="AN31" s="7"/>
       <c r="AO31" s="7"/>
     </row>
-    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A34" s="1"/>
       <c r="B34" s="2" t="s">
         <v>4</v>
@@ -3056,7 +3235,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
         <v>41</v>
       </c>
@@ -3073,7 +3252,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A38" s="1"/>
       <c r="B38" s="2" t="s">
         <v>1</v>
@@ -3088,7 +3267,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
         <v>44</v>
       </c>
@@ -3105,13 +3284,13 @@
         <v>43</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A42" s="1"/>
       <c r="B42" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
         <v>46</v>
       </c>
@@ -3119,7 +3298,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A46" s="1"/>
       <c r="B46" s="2" t="s">
         <v>5</v>
@@ -3128,7 +3307,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A47" s="1" t="s">
         <v>48</v>
       </c>
@@ -3139,7 +3318,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A50" s="1"/>
       <c r="B50" s="2" t="s">
         <v>7</v>
@@ -3154,7 +3333,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A51" s="1" t="s">
         <v>50</v>
       </c>
@@ -3171,7 +3350,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A54" s="1"/>
       <c r="B54" s="2" t="s">
         <v>12</v>
@@ -3183,7 +3362,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A55" s="1" t="s">
         <v>52</v>
       </c>
@@ -3197,7 +3376,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A58" s="1"/>
       <c r="B58" s="2" t="s">
         <v>15</v>
@@ -3209,7 +3388,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A59" s="1" t="s">
         <v>53</v>
       </c>
@@ -3223,7 +3402,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A62" s="1"/>
       <c r="B62" s="2" t="s">
         <v>15</v>
@@ -3232,7 +3411,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A63" s="1" t="s">
         <v>55</v>
       </c>
@@ -3243,13 +3422,13 @@
         <v>57</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A66" s="1"/>
       <c r="B66" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A67" s="1" t="s">
         <v>58</v>
       </c>
@@ -3257,7 +3436,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A70" s="1"/>
       <c r="B70" s="2" t="s">
         <v>1</v>
@@ -3281,7 +3460,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A71" s="1" t="s">
         <v>60</v>
       </c>
@@ -3307,7 +3486,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A74" s="1"/>
       <c r="B74" s="2" t="s">
         <v>1</v>
@@ -3328,7 +3507,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A75" s="1" t="s">
         <v>62</v>
       </c>
@@ -3339,33 +3518,33 @@
         <v>59</v>
       </c>
       <c r="D75" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E75" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E75" s="2" t="s">
+      <c r="F75" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F75" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="G75" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A78" s="1"/>
       <c r="B78" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A79" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A82" s="1"/>
       <c r="B82" s="2" t="s">
         <v>2</v>
@@ -3374,44 +3553,38 @@
         <v>8</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E82" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A83" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C83" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B83" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C83" s="2" t="s">
+      <c r="D83" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D83" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E83" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A86" s="1"/>
       <c r="B86" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A87" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B87" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B87" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A90" s="1"/>
       <c r="B90" s="2" t="s">
         <v>2</v>
@@ -3426,40 +3599,37 @@
         <v>20</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G90" s="2" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="H90" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I90" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J90" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K90" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="L90" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="M90" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A91" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C91" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B91" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C91" s="2" t="s">
-        <v>74</v>
-      </c>
       <c r="D91" s="1" t="s">
         <v>43</v>
       </c>
@@ -3487,11 +3657,8 @@
       <c r="L91" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="M91" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A94" s="1"/>
       <c r="B94" s="2" t="s">
         <v>25</v>
@@ -3500,18 +3667,18 @@
         <v>26</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A95" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B95" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C95" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C95" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="98" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A98" s="1"/>
       <c r="B98" s="2" t="s">
         <v>1</v>
@@ -3528,8 +3695,8 @@
       <c r="F98" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G98" s="3" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="G98" s="3" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H98" s="2" t="s">
@@ -3539,36 +3706,36 @@
         <v>37</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A99" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B99" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B99" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="C99" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I99" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="102" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A102" s="1"/>
       <c r="B102" s="2" t="s">
         <v>2</v>
@@ -3577,42 +3744,36 @@
         <v>20</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G102" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A103" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F103" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B103" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C103" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D103" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E103" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F103" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G103" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="106" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A106" s="1"/>
       <c r="B106" s="2" t="s">
         <v>1</v>
@@ -3629,8 +3790,8 @@
       <c r="F106" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G106" s="3" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="G106" s="3" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="H106" s="2" t="s">
@@ -3640,36 +3801,36 @@
         <v>37</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A107" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B107" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B107" s="1" t="s">
+      <c r="C107" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G107" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H107" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C107" s="1" t="s">
+      <c r="I107" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D107" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E107" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="F107" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="G107" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="H107" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="I107" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="110" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A110" s="1"/>
       <c r="B110" s="2" t="s">
         <v>2</v>
@@ -3681,57 +3842,51 @@
         <v>20</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="G110" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H110" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I110" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J110" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A111" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G111" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H111" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="B111" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C111" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D111" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E111" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F111" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G111" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H111" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="I111" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="J111" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="114" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A114" s="1"/>
       <c r="B114" s="2" t="s">
         <v>1</v>
@@ -3748,35 +3903,35 @@
       <c r="F114" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G114" s="3" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="G114" s="3" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A115" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B115" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B115" s="1" t="s">
-        <v>88</v>
-      </c>
       <c r="C115" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G115" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="118" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A118" s="1"/>
       <c r="B118" s="2" t="s">
         <v>2</v>
@@ -3788,69 +3943,63 @@
         <v>20</v>
       </c>
       <c r="E118" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F118" s="2" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="G118" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H118" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I118" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J118" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K118" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="L118" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A119" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F119" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G119" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H119" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I119" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J119" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="B119" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C119" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D119" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E119" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F119" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G119" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H119" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="I119" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J119" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="K119" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="L119" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="122" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A122" s="1"/>
       <c r="B122" s="2" t="s">
         <v>1</v>
@@ -3867,26 +4016,26 @@
       <c r="F122" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G122" s="3" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="G122" s="3" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
     </row>
-    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A123" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C123" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D123" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E123" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="E123" s="2" t="s">
-        <v>94</v>
       </c>
       <c r="F123" s="2" t="s">
         <v>35</v>
@@ -3895,7 +4044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A126" s="1"/>
       <c r="B126" s="2" t="s">
         <v>36</v>
@@ -3904,9 +4053,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="127" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A127" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B127" s="2" t="s">
         <v>36</v>
@@ -3916,10 +4065,9 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPágina &amp;P</oddFooter>
   </headerFooter>

</xml_diff>